<commit_message>
Update backlogs to include more details
</commit_message>
<xml_diff>
--- a/project-planning/ph1-inception/artifacts/SCRUM_Backlogs.xlsx
+++ b/project-planning/ph1-inception/artifacts/SCRUM_Backlogs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8231DE13-4894-4D07-8FE0-06C2E5D2C619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DE45EB-976C-4E29-A9BF-46F9FFADCE7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -117,43 +117,73 @@
     <t>Person(s)</t>
   </si>
   <si>
-    <t>As a student I want to upload files (PDF, DOCX, plain text).</t>
-  </si>
-  <si>
     <t>Planned</t>
   </si>
   <si>
-    <t>As a student I want the text from uploaded files to be preprocessed (cleaning, segmentation).</t>
-  </si>
-  <si>
-    <t>As a student I want uploaded files to be summarized using pre-trained open-source models (e.g. BART, T5).</t>
-  </si>
-  <si>
-    <t>As a student I want questions to be generated for flashcards and quizzes.</t>
-  </si>
-  <si>
-    <t>As a student I want to be able to use interactive quizes/flashcards.</t>
-  </si>
-  <si>
-    <t>As a student I want my progress to be tracked (score history, completed sets)</t>
-  </si>
-  <si>
-    <t>As a student I want an user account for saving study sessions.</t>
-  </si>
-  <si>
-    <t>As a student I want to be able to publish and share flashcards and quizzes.</t>
-  </si>
-  <si>
     <t>As a university I want to create and manage an organization for students to be connected to.</t>
   </si>
   <si>
-    <t>As a student I want to be able to use an exam mode.</t>
-  </si>
-  <si>
     <t>Exam mode would simulate an exam and provide information about the amount of time spend on each part. Possibly includes a pause feature.</t>
   </si>
   <si>
-    <t>As a student I want to be able to work with multiple languages</t>
+    <t>Accept PDF, DOCX, and TXT files that are up to a certain size limit. (E.X. XXX KB)</t>
+  </si>
+  <si>
+    <t>As a student I want to upload lecture materials/notes to the website for studying.</t>
+  </si>
+  <si>
+    <t>As a student I want my uploaded notes to be processed and summarized by NLP model.</t>
+  </si>
+  <si>
+    <t>This would involve text processesing such as text cleaning and segmentation. The NLP model should be open source.</t>
+  </si>
+  <si>
+    <t>As a student I want flashcards and quizzes to be generated for my uploaded materials to use for studying.</t>
+  </si>
+  <si>
+    <t>As a student I want interactive modes to allow me to effectively utilize the generated flashcards and quizzes.</t>
+  </si>
+  <si>
+    <t>An example of what these modes could look like is Quizlet.</t>
+  </si>
+  <si>
+    <t>As a student I want to track my progress and performance to understand what I need to work on the most.</t>
+  </si>
+  <si>
+    <t>As a student I want to have an account to save generated flashcards/quizzes and see overall statistics.</t>
+  </si>
+  <si>
+    <t>As a student I want to be able to publish and share my generated flashcards and quizzes.</t>
+  </si>
+  <si>
+    <t>This could involve sharing to an invidiual student, to the entire university, or to every user.</t>
+  </si>
+  <si>
+    <t>As an international student I want to be able to be able to use the website in multiple languages to allow me to study in my native language.</t>
+  </si>
+  <si>
+    <t>We should at least add a framework so it would be easy to add more languages to the website.</t>
+  </si>
+  <si>
+    <t>As a student I want to be able to use an exam mode to prepare for class exams.</t>
+  </si>
+  <si>
+    <t>As a student/university I want to be able to use/publish additional functionality from a plugin marketplace to improve my studying experience.</t>
+  </si>
+  <si>
+    <t>Examples of plugins could include additional AI models, such as ones trained for specific subjects or languages.</t>
+  </si>
+  <si>
+    <t>As a student I want to be able to chat with an AI agent for explanations about topics I don't fully understand</t>
+  </si>
+  <si>
+    <t>Should be able to answer questions about topics from the provided/generated materials (Like the AI in textbook websites). Possibly allow it to see your statistics to give it context on the level of the person asking. This AI should have some level of memory to be able to at least answer follow up questions, there is a possibility to save chat instances so a student can return to a topic they asked about.</t>
+  </si>
+  <si>
+    <t>As a student I want to be able to export the generated content for use outside of the website.</t>
+  </si>
+  <si>
+    <t>For use in making physical flashcards or doing a quiz on paper exporting to PDF would be the best option, if we want to allow importing of quizzes and flashcards we can create a JSON format for them.</t>
   </si>
 </sst>
 </file>
@@ -353,11 +383,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -367,20 +412,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -388,6 +424,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -396,15 +435,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -710,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="D6" sqref="D6:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -760,32 +790,38 @@
       <c r="F2" s="21"/>
       <c r="G2" s="20"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -793,13 +829,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -807,13 +843,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -821,13 +860,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -835,41 +874,44 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>38</v>
+      <c r="B9" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="C9" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -877,44 +919,84 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C11" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C12" s="2">
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C13" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>42</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="2">
+        <v>5</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -995,12 +1077,12 @@
       <c r="B8" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="31"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="28"/>
       <c r="G8" s="18" t="s">
         <v>3</v>
       </c>
@@ -1012,12 +1094,12 @@
       <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="31"/>
       <c r="G9" s="2" t="s">
         <v>23</v>
       </c>
@@ -1025,10 +1107,10 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="31"/>
       <c r="G10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1047,10 +1129,10 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="31"/>
       <c r="G12" s="2" t="s">
         <v>26</v>
       </c>
@@ -1061,38 +1143,38 @@
       </c>
     </row>
     <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="24" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>20</v>
       </c>
       <c r="E15" s="20"/>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="24" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="23"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="19" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
@@ -1384,16 +1466,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="D15:E15"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="C8:F8"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="D15:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1461,12 +1543,12 @@
       <c r="B8" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="36"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="15" t="s">
         <v>3</v>
       </c>
@@ -1474,19 +1556,19 @@
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="31"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="31"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1501,10 +1583,10 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="31"/>
       <c r="G12" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1513,38 +1595,38 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="32" t="s">
+      <c r="E15" s="36"/>
+      <c r="F15" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="32" t="s">
+      <c r="G15" s="34" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="38"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="33"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="16" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
@@ -1800,16 +1882,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C12:F12"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>